<commit_message>
Include Neo4j dependencies in pom file
</commit_message>
<xml_diff>
--- a/output/recipes_1.7k_20240119.xlsx
+++ b/output/recipes_1.7k_20240119.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6CABE6F3-F25B-45BA-82F5-DB9C0DD0D1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="recipes_1.7k_20240119" sheetId="1" r:id="rId1"/>
@@ -10600,7 +10600,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -11449,13 +11449,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1762"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="B166" sqref="B166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30848,7 +30848,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1762"/>
+  <autoFilter ref="A1:C1762" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>